<commit_message>
Characteristic 'Matryoshka' bug seemingly fixed
Previously, if characteristic a had an entry point included in b and b
had an entry point included in c, then model.py would extract a from b
and BOTH a and b from c.
This meant that a would be double-counted, e.g. 5k SP cases subtracted
from 10k active cases AND subtracted from 20k living people, resulting
in an incorrect 5k:5k:5k split rather than the correct 5k:5k:10k
partition for SP:Act:Alive.
The code in model.py now hopefully fixes this by determining the
smallest enclosing sets for each entry point, so that extractions work
much like a Matryoshka doll.
</commit_message>
<xml_diff>
--- a/data/cascade.xlsx
+++ b/data/cascade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="410">
   <si>
     <t>Code Label</t>
   </si>
@@ -1236,6 +1236,18 @@
   </si>
   <si>
     <t>check+check</t>
+  </si>
+  <si>
+    <t>spd_prev</t>
+  </si>
+  <si>
+    <t>SP DS Prevalence</t>
+  </si>
+  <si>
+    <t>snd_prev</t>
+  </si>
+  <si>
+    <t>SN DS Prevalence</t>
   </si>
 </sst>
 </file>
@@ -3862,10 +3874,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4179,6 +4191,9 @@
       <c r="C13" s="2" t="s">
         <v>161</v>
       </c>
+      <c r="E13" s="2">
+        <v>0.2</v>
+      </c>
       <c r="F13" s="2" t="s">
         <v>114</v>
       </c>
@@ -4324,8 +4339,7 @@
         <v>161</v>
       </c>
       <c r="E20" s="2">
-        <f>10000/E12</f>
-        <v>0.01</v>
+        <v>0.2</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>114</v>
@@ -4350,6 +4364,9 @@
       <c r="C21" s="2" t="s">
         <v>161</v>
       </c>
+      <c r="E21" s="2">
+        <v>0.3</v>
+      </c>
       <c r="F21" s="2" t="s">
         <v>114</v>
       </c>
@@ -4370,17 +4387,78 @@
       <c r="B22" t="s">
         <v>131</v>
       </c>
-      <c r="D22" s="2">
-        <v>-1</v>
+      <c r="E22" s="2">
+        <v>0.7</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="G22" s="2" t="s">
+        <v>336</v>
+      </c>
       <c r="H22" t="s">
         <v>120</v>
       </c>
       <c r="I22" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>406</v>
+      </c>
+      <c r="B23" t="s">
+        <v>407</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="H23" t="s">
+        <v>120</v>
+      </c>
+      <c r="I23" t="s">
+        <v>240</v>
+      </c>
+      <c r="J23" t="s">
+        <v>241</v>
+      </c>
+      <c r="K23" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>408</v>
+      </c>
+      <c r="B24" t="s">
+        <v>409</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="H24" t="s">
+        <v>120</v>
+      </c>
+      <c r="I24" t="s">
+        <v>249</v>
+      </c>
+      <c r="J24" t="s">
+        <v>250</v>
+      </c>
+      <c r="K24" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -4393,7 +4471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>